<commit_message>
optimized code for friend node
The code was developed together with my teammates (Om Raheja and Amogh Shrikhande)
</commit_message>
<xml_diff>
--- a/command_table/Mesh_Project_Command_Table.xlsx
+++ b/command_table/Mesh_Project_Command_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\SimplicityStudio\v4_workspace\ecen5823-mesh-assignment\assignment-10-bluetooth-mesh-MohitRane8\command_table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2B9BFC-BDBB-400C-9060-F6053A7878B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6B9B4-A208-44EC-9DAA-52F832A4B51D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mesh Project Command Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -76,30 +76,6 @@
     <t>gecko_evt_mesh_node_initialized_id</t>
   </si>
   <si>
-    <t>provisioned &amp;&amp; DeviceUsesClientModel()</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceUsesServerModel()</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,8)</t>
-  </si>
-  <si>
-    <t>Initialize the mesh library with support of up to 8 models</t>
-  </si>
-  <si>
-    <t>provisioned &amp;&amp; DeviceIsOnOffSubscriber()</t>
-  </si>
-  <si>
-    <t>mesh_lib_init(malloc,free,9), mesh_lib_generic_server_register_handler, mesh_lib_generic_server_update, mesh_lib_generic_server_publish</t>
-  </si>
-  <si>
-    <t>See init_models, onoff_request, onoff_update_and_publish in lightbulb.c, soc-btmesh-light example</t>
-  </si>
-  <si>
     <t>!provisioned</t>
   </si>
   <si>
@@ -133,9 +109,6 @@
     <t>gecko_evt_mesh_generic_server_client_request_id</t>
   </si>
   <si>
-    <t>DeviceUsesServerModel()</t>
-  </si>
-  <si>
     <t>mesh_lib_generic_server_event_handler</t>
   </si>
   <si>
@@ -166,109 +139,44 @@
     <t>Handle scheduler events</t>
   </si>
   <si>
-    <t>Button 0 press or release event &amp;&amp; DeviceIsOnOffPublisher()</t>
-  </si>
-  <si>
-    <t>mesh_lib_generic_client_publish</t>
-  </si>
-  <si>
-    <t>Publish button press or release using the on off model.  Press = on</t>
-  </si>
-  <si>
-    <t>client request or server change callback for generic on/off model</t>
-  </si>
-  <si>
-    <t>"Button Pressed" or "Button Released"</t>
-  </si>
-  <si>
-    <t>Display the state of the button on the subscriber</t>
-  </si>
-  <si>
     <t>SetDeviceName; gecko_cmd_mesh_node_init</t>
   </si>
   <si>
-    <t>factory reset timer handle, display update timer handle, log time timer handle, friend find timer handle</t>
-  </si>
-  <si>
     <t>Completes factory reset, updates display for remove charge buildup, log timestamp value increase, tries to establish friendship on Client side</t>
   </si>
   <si>
-    <t>gecko_evt_mesh_lpn_friendship_established_id</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_generic_server_init, gecko_cmd_mesh_friend_init()</t>
-  </si>
-  <si>
     <t>Initialize the client model and does low power node initialization</t>
   </si>
   <si>
-    <t>Initialize the server model and friend initialization</t>
-  </si>
-  <si>
-    <t>gecko_evt_mesh_lpn_friendship_failed_id</t>
-  </si>
-  <si>
-    <t>gecko_evt_mesh_lpn_friendship_terminated_id</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_lpn_establish_friendship(0)</t>
-  </si>
-  <si>
-    <t>gecko_cmd_hardware_set_soft_timer</t>
-  </si>
-  <si>
     <t>DISPLAY_ROW_LPN update</t>
   </si>
   <si>
-    <t>LPN</t>
-  </si>
-  <si>
-    <t>no friend</t>
-  </si>
-  <si>
-    <t>friend lost</t>
-  </si>
-  <si>
-    <t>Friendship is established when this node</t>
-  </si>
-  <si>
-    <t>Tries to establish friendship every 2 seconds until it is established</t>
-  </si>
-  <si>
     <t>gecko_cmd_system_reset, displayUpdate, gecko_cmd_mesh_lpn_establish_friendship (only for LPN)</t>
   </si>
   <si>
-    <t>gecko_evt_mesh_lpn_friendship_established_id, gecko_evt_mesh_lpn_friendship_failed_id (only for LPN)</t>
-  </si>
-  <si>
-    <t>gecko_cmd_mesh_generic_client_init, lpn_init, gpioIntEnable</t>
-  </si>
-  <si>
-    <t>This node will implement the Server model (friend node)</t>
-  </si>
-  <si>
     <t>NOTE: This command table might be updated in future and code will be done accordingly. For now code is written such that it is capable of implementing both server and client functionality, however, the unrequired code will be removed in future.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">On LPN side (2 nodes) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(unused at this node)</t>
-    </r>
+    <t>This node will implement the Client model (friend node)</t>
+  </si>
+  <si>
+    <t>factory reset timer handle, display update timer handle, log time timer handle, friend find timer handle, ir1, ir2 and vibration timer handle, vibration local alert</t>
+  </si>
+  <si>
+    <t>gecko_cmd_mesh_generic_client_init, friend_init, gpioIntEnable, mesh_lib_init(malloc,free,8)</t>
+  </si>
+  <si>
+    <t>on vibration, pb0 and IR sensor interrupt</t>
+  </si>
+  <si>
+    <t>mesh_lib_generic_client_publish (in pb0 and vibration case)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -298,12 +206,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -341,11 +243,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,28 +565,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="6" width="33.21875" customWidth="1"/>
-    <col min="7" max="8" width="51.44140625" customWidth="1"/>
+    <col min="1" max="1" width="34.3515625" customWidth="1"/>
+    <col min="2" max="2" width="36.64453125" customWidth="1"/>
+    <col min="3" max="3" width="31.52734375" customWidth="1"/>
+    <col min="4" max="4" width="31.64453125" customWidth="1"/>
+    <col min="5" max="6" width="33.234375" customWidth="1"/>
+    <col min="7" max="8" width="51.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
@@ -710,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -732,7 +634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -740,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -752,35 +654,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>72</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>73</v>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
@@ -789,339 +687,187 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+        <v>20</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="1" t="s">
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A30:C32"/>
+    <mergeCell ref="A20:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>